<commit_message>
Add ppp aggregates csv
</commit_message>
<xml_diff>
--- a/app/static/data/ppp_aggregate_data.xlsx
+++ b/app/static/data/ppp_aggregate_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rishan\Google Drive\Github\bs-table\app\static\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D60293CD-D4E9-4CFC-AF5F-1BC74AE11327}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A68023EC-B7CD-4359-8B36-4F1C5506412C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2184" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2184" uniqueCount="223">
   <si>
     <t>state</t>
   </si>
@@ -685,6 +685,21 @@
   </si>
   <si>
     <t>$/job</t>
+  </si>
+  <si>
+    <t>totaljobs</t>
+  </si>
+  <si>
+    <t>totalloanamount</t>
+  </si>
+  <si>
+    <t>loancountnojobs</t>
+  </si>
+  <si>
+    <t>totalloansnojobs</t>
+  </si>
+  <si>
+    <t>avgloansizenojobs</t>
   </si>
 </sst>
 </file>
@@ -6844,10 +6859,10 @@
   <dimension ref="A1:J59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" sqref="A1:J59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6872,10 +6887,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>218</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>219</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -6887,13 +6902,13 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>65</v>
+        <v>220</v>
       </c>
       <c r="I1" t="s">
-        <v>66</v>
+        <v>221</v>
       </c>
       <c r="J1" t="s">
-        <v>67</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add all data columns, data, and footers to summary table
</commit_message>
<xml_diff>
--- a/app/static/data/ppp_aggregate_data.xlsx
+++ b/app/static/data/ppp_aggregate_data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rishan\Google Drive\Github\bs-table\app\static\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A68023EC-B7CD-4359-8B36-4F1C5506412C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A361143-B03A-413B-A986-0719D37A234A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5"/>
+    <workbookView xWindow="7200" yWindow="-21045" windowWidth="23580" windowHeight="18315" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined" sheetId="6" r:id="rId1"/>
@@ -18,20 +18,33 @@
     <sheet name="Data2" sheetId="2" r:id="rId3"/>
     <sheet name="Data3" sheetId="3" r:id="rId4"/>
     <sheet name="Data4" sheetId="5" r:id="rId5"/>
-    <sheet name="Combined_Hardcoded" sheetId="7" r:id="rId6"/>
-    <sheet name="NULL data" sheetId="8" r:id="rId7"/>
-    <sheet name="NULL data summary" sheetId="9" r:id="rId8"/>
+    <sheet name="Sums" sheetId="11" r:id="rId6"/>
+    <sheet name="Combined_Hardcoded" sheetId="7" r:id="rId7"/>
+    <sheet name="NULL data aggregate" sheetId="10" r:id="rId8"/>
+    <sheet name="NULL data" sheetId="8" r:id="rId9"/>
+    <sheet name="NULL data summary" sheetId="9" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Combined_Hardcoded!$A$1:$J$59</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'NULL data'!$A$1:$P$139</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Combined_Hardcoded!$A$1:$J$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'NULL data'!$A$1:$P$139</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2184" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2252" uniqueCount="230">
   <si>
     <t>state</t>
   </si>
@@ -700,19 +713,40 @@
   </si>
   <si>
     <t>avgloansizenojobs</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Null $ / job</t>
+  </si>
+  <si>
+    <t>Null Jobs per Loan</t>
+  </si>
+  <si>
+    <t>totalnullamount</t>
+  </si>
+  <si>
+    <t>totalnullloans</t>
+  </si>
+  <si>
+    <t>totalnulljobs</t>
+  </si>
+  <si>
+    <t>Excludes null jobs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1199,15 +1233,20 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="21" builtinId="30" customBuiltin="1"/>
@@ -1564,7 +1603,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4003,8 +4042,1336 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A2:S141"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S4" sqref="S4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>213</v>
+      </c>
+      <c r="L2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E3" t="s">
+        <v>207</v>
+      </c>
+      <c r="F3" t="s">
+        <v>208</v>
+      </c>
+      <c r="G3" t="s">
+        <v>209</v>
+      </c>
+      <c r="H3" t="s">
+        <v>217</v>
+      </c>
+      <c r="J3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L3" t="s">
+        <v>210</v>
+      </c>
+      <c r="M3" t="s">
+        <v>211</v>
+      </c>
+      <c r="N3" t="s">
+        <v>212</v>
+      </c>
+      <c r="P3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>148440</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <f>COUNT(A4:A41)</f>
+        <v>38</v>
+      </c>
+      <c r="E4" s="1">
+        <f>SUM(A4:A41)</f>
+        <v>2070510</v>
+      </c>
+      <c r="F4" s="4">
+        <f>SUM(B4:B41)</f>
+        <v>220</v>
+      </c>
+      <c r="G4" s="2">
+        <f>F4/D4</f>
+        <v>5.7894736842105265</v>
+      </c>
+      <c r="H4" s="5">
+        <f>E4/F4</f>
+        <v>9411.4090909090901</v>
+      </c>
+      <c r="J4" s="1">
+        <v>148440</v>
+      </c>
+      <c r="L4" s="1">
+        <f>SUM(J4:J141)</f>
+        <v>6030063</v>
+      </c>
+      <c r="M4">
+        <f>COUNT(J4:J141)</f>
+        <v>138</v>
+      </c>
+      <c r="N4" s="1">
+        <f>L4/M4</f>
+        <v>43696.108695652176</v>
+      </c>
+      <c r="P4" s="1">
+        <v>109988</v>
+      </c>
+      <c r="R4" s="1">
+        <f>SUM(P4:P103)</f>
+        <v>3959553</v>
+      </c>
+      <c r="S4">
+        <f>COUNT(P4:P103)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>128440</v>
+      </c>
+      <c r="B5">
+        <v>9</v>
+      </c>
+      <c r="J5" s="1">
+        <v>128440</v>
+      </c>
+      <c r="P5" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>111200</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="J6" s="1">
+        <v>111200</v>
+      </c>
+      <c r="P6" s="1">
+        <v>89241</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>90394</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="J7" s="1">
+        <v>109988</v>
+      </c>
+      <c r="P7" s="1">
+        <v>87886</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>62398</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="J8" s="1">
+        <v>100000</v>
+      </c>
+      <c r="P8" s="1">
+        <v>80260</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>61711</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="J9" s="1">
+        <v>90394</v>
+      </c>
+      <c r="P9" s="1">
+        <v>79003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>60320</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="J10" s="1">
+        <v>89241</v>
+      </c>
+      <c r="P10" s="1">
+        <v>76871</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>52861</v>
+      </c>
+      <c r="B11">
+        <v>14</v>
+      </c>
+      <c r="J11" s="1">
+        <v>87886</v>
+      </c>
+      <c r="P11" s="1">
+        <v>57430</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>52605</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="J12" s="1">
+        <v>80260</v>
+      </c>
+      <c r="P12" s="1">
+        <v>49563</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>49207</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="J13" s="1">
+        <v>79003</v>
+      </c>
+      <c r="P13" s="1">
+        <v>43168</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>44129</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="J14" s="1">
+        <v>76871</v>
+      </c>
+      <c r="P14" s="1">
+        <v>41668</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>37582</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="J15" s="1">
+        <v>62398</v>
+      </c>
+      <c r="P15" s="1">
+        <v>41500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>37500</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="J16" s="1">
+        <v>61711</v>
+      </c>
+      <c r="P16" s="1">
+        <v>41153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>33233</v>
+      </c>
+      <c r="B17">
+        <v>12</v>
+      </c>
+      <c r="J17" s="1">
+        <v>60320</v>
+      </c>
+      <c r="P17" s="1">
+        <v>36723</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>30000</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="J18" s="1">
+        <v>57430</v>
+      </c>
+      <c r="P18" s="1">
+        <v>34188</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>22455</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="J19" s="1">
+        <v>52861</v>
+      </c>
+      <c r="P19" s="1">
+        <v>32625</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>21815</v>
+      </c>
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="J20" s="1">
+        <v>52605</v>
+      </c>
+      <c r="P20" s="1">
+        <v>31340</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>21051</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="J21" s="1">
+        <v>49563</v>
+      </c>
+      <c r="P21" s="1">
+        <v>30824</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>20274</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="J22" s="1">
+        <v>49207</v>
+      </c>
+      <c r="P22" s="1">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>16467</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="J23" s="1">
+        <v>44129</v>
+      </c>
+      <c r="P23" s="1">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>16385</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="J24" s="1">
+        <v>43168</v>
+      </c>
+      <c r="P24" s="1">
+        <v>27684</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>15000</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="J25" s="1">
+        <v>41668</v>
+      </c>
+      <c r="P25" s="1">
+        <v>27427</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>12572</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="J26" s="1">
+        <v>41500</v>
+      </c>
+      <c r="P26" s="1">
+        <v>27275</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>10415</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="J27" s="1">
+        <v>41153</v>
+      </c>
+      <c r="P27" s="1">
+        <v>25762</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>6352</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="J28" s="1">
+        <v>37582</v>
+      </c>
+      <c r="P28" s="1">
+        <v>23968</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>5923</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="J29" s="1">
+        <v>37500</v>
+      </c>
+      <c r="P29" s="1">
+        <v>23021</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>5495</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="J30" s="1">
+        <v>36723</v>
+      </c>
+      <c r="P30" s="1">
+        <v>22528</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>3854</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="J31" s="1">
+        <v>34188</v>
+      </c>
+      <c r="P31" s="1">
+        <v>22500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>3748</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="J32" s="1">
+        <v>33233</v>
+      </c>
+      <c r="P32" s="1">
+        <v>22500</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>2500</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="J33" s="1">
+        <v>32625</v>
+      </c>
+      <c r="P33" s="1">
+        <v>22200</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>2445</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="J34" s="1">
+        <v>31340</v>
+      </c>
+      <c r="P34" s="1">
+        <v>21813</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>2302</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="J35" s="1">
+        <v>30824</v>
+      </c>
+      <c r="P35" s="1">
+        <v>21250</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>1987</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="J36" s="1">
+        <v>30000</v>
+      </c>
+      <c r="P36" s="1">
+        <v>20833</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>1332</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="J37" s="1">
+        <v>30000</v>
+      </c>
+      <c r="P37" s="1">
+        <v>20833</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>267035</v>
+      </c>
+      <c r="B38">
+        <v>16</v>
+      </c>
+      <c r="J38" s="1">
+        <v>30000</v>
+      </c>
+      <c r="P38" s="1">
+        <v>20833</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>219537</v>
+      </c>
+      <c r="B39">
+        <v>17</v>
+      </c>
+      <c r="J39" s="1">
+        <v>27684</v>
+      </c>
+      <c r="P39" s="1">
+        <v>20833</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>217500</v>
+      </c>
+      <c r="B40">
+        <v>14</v>
+      </c>
+      <c r="J40" s="1">
+        <v>27427</v>
+      </c>
+      <c r="P40" s="1">
+        <v>20833</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>174046</v>
+      </c>
+      <c r="B41">
+        <v>18</v>
+      </c>
+      <c r="J41" s="1">
+        <v>27275</v>
+      </c>
+      <c r="P41" s="1">
+        <v>20691</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J42" s="1">
+        <v>25762</v>
+      </c>
+      <c r="P42" s="1">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J43" s="1">
+        <v>23968</v>
+      </c>
+      <c r="P43" s="1">
+        <v>19353</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J44" s="1">
+        <v>23021</v>
+      </c>
+      <c r="P44" s="1">
+        <v>18203</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J45" s="1">
+        <v>22528</v>
+      </c>
+      <c r="P45" s="1">
+        <v>17693</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J46" s="1">
+        <v>22500</v>
+      </c>
+      <c r="P46" s="1">
+        <v>17500</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J47" s="1">
+        <v>22500</v>
+      </c>
+      <c r="P47" s="1">
+        <v>17500</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J48" s="1">
+        <v>22455</v>
+      </c>
+      <c r="P48" s="1">
+        <v>17415</v>
+      </c>
+    </row>
+    <row r="49" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J49" s="1">
+        <v>22200</v>
+      </c>
+      <c r="P49" s="1">
+        <v>17000</v>
+      </c>
+    </row>
+    <row r="50" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J50" s="1">
+        <v>21815</v>
+      </c>
+      <c r="P50" s="1">
+        <v>16968</v>
+      </c>
+    </row>
+    <row r="51" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J51" s="1">
+        <v>21813</v>
+      </c>
+      <c r="P51" s="1">
+        <v>16873</v>
+      </c>
+    </row>
+    <row r="52" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J52" s="1">
+        <v>21250</v>
+      </c>
+      <c r="P52" s="1">
+        <v>16350</v>
+      </c>
+    </row>
+    <row r="53" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J53" s="1">
+        <v>21051</v>
+      </c>
+      <c r="P53" s="1">
+        <v>16115</v>
+      </c>
+    </row>
+    <row r="54" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J54" s="1">
+        <v>20833</v>
+      </c>
+      <c r="P54" s="1">
+        <v>15960</v>
+      </c>
+    </row>
+    <row r="55" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J55" s="1">
+        <v>20833</v>
+      </c>
+      <c r="P55" s="1">
+        <v>15870</v>
+      </c>
+    </row>
+    <row r="56" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J56" s="1">
+        <v>20833</v>
+      </c>
+      <c r="P56" s="1">
+        <v>15625</v>
+      </c>
+    </row>
+    <row r="57" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J57" s="1">
+        <v>20833</v>
+      </c>
+      <c r="P57" s="1">
+        <v>15433</v>
+      </c>
+    </row>
+    <row r="58" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J58" s="1">
+        <v>20833</v>
+      </c>
+      <c r="P58" s="1">
+        <v>15291</v>
+      </c>
+    </row>
+    <row r="59" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J59" s="1">
+        <v>20691</v>
+      </c>
+      <c r="P59" s="1">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="60" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J60" s="1">
+        <v>20274</v>
+      </c>
+      <c r="P60" s="1">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="61" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J61" s="1">
+        <v>20000</v>
+      </c>
+      <c r="P61" s="1">
+        <v>14603</v>
+      </c>
+    </row>
+    <row r="62" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J62" s="1">
+        <v>19353</v>
+      </c>
+      <c r="P62" s="1">
+        <v>14543</v>
+      </c>
+    </row>
+    <row r="63" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J63" s="1">
+        <v>18203</v>
+      </c>
+      <c r="P63" s="1">
+        <v>14282</v>
+      </c>
+    </row>
+    <row r="64" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J64" s="1">
+        <v>17693</v>
+      </c>
+      <c r="P64" s="1">
+        <v>13168</v>
+      </c>
+    </row>
+    <row r="65" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J65" s="1">
+        <v>17500</v>
+      </c>
+      <c r="P65" s="1">
+        <v>13148</v>
+      </c>
+    </row>
+    <row r="66" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J66" s="1">
+        <v>17500</v>
+      </c>
+      <c r="P66" s="1">
+        <v>11789</v>
+      </c>
+    </row>
+    <row r="67" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J67" s="1">
+        <v>17415</v>
+      </c>
+      <c r="P67" s="1">
+        <v>11581</v>
+      </c>
+    </row>
+    <row r="68" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J68" s="1">
+        <v>17000</v>
+      </c>
+      <c r="P68" s="1">
+        <v>11250</v>
+      </c>
+    </row>
+    <row r="69" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J69" s="1">
+        <v>16968</v>
+      </c>
+      <c r="P69" s="1">
+        <v>10954</v>
+      </c>
+    </row>
+    <row r="70" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J70" s="1">
+        <v>16873</v>
+      </c>
+      <c r="P70" s="1">
+        <v>10816</v>
+      </c>
+    </row>
+    <row r="71" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J71" s="1">
+        <v>16467</v>
+      </c>
+      <c r="P71" s="1">
+        <v>9818</v>
+      </c>
+    </row>
+    <row r="72" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J72" s="1">
+        <v>16385</v>
+      </c>
+      <c r="P72" s="1">
+        <v>9700</v>
+      </c>
+    </row>
+    <row r="73" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J73" s="1">
+        <v>16350</v>
+      </c>
+      <c r="P73" s="1">
+        <v>9500</v>
+      </c>
+    </row>
+    <row r="74" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J74" s="1">
+        <v>16115</v>
+      </c>
+      <c r="P74" s="1">
+        <v>9076</v>
+      </c>
+    </row>
+    <row r="75" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J75" s="1">
+        <v>15960</v>
+      </c>
+      <c r="P75" s="1">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="76" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J76" s="1">
+        <v>15870</v>
+      </c>
+      <c r="P76" s="1">
+        <v>8750</v>
+      </c>
+    </row>
+    <row r="77" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J77" s="1">
+        <v>15625</v>
+      </c>
+      <c r="P77" s="1">
+        <v>8750</v>
+      </c>
+    </row>
+    <row r="78" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J78" s="1">
+        <v>15433</v>
+      </c>
+      <c r="P78" s="1">
+        <v>8542</v>
+      </c>
+    </row>
+    <row r="79" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J79" s="1">
+        <v>15291</v>
+      </c>
+      <c r="P79" s="1">
+        <v>8380</v>
+      </c>
+    </row>
+    <row r="80" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J80" s="1">
+        <v>15000</v>
+      </c>
+      <c r="P80" s="1">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="81" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J81" s="1">
+        <v>15000</v>
+      </c>
+      <c r="P81" s="1">
+        <v>7993</v>
+      </c>
+    </row>
+    <row r="82" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J82" s="1">
+        <v>15000</v>
+      </c>
+      <c r="P82" s="1">
+        <v>7086</v>
+      </c>
+    </row>
+    <row r="83" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J83" s="1">
+        <v>14603</v>
+      </c>
+      <c r="P83" s="1">
+        <v>7060</v>
+      </c>
+    </row>
+    <row r="84" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J84" s="1">
+        <v>14543</v>
+      </c>
+      <c r="P84" s="1">
+        <v>6875</v>
+      </c>
+    </row>
+    <row r="85" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J85" s="1">
+        <v>14282</v>
+      </c>
+      <c r="P85" s="1">
+        <v>6834</v>
+      </c>
+    </row>
+    <row r="86" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J86" s="1">
+        <v>13168</v>
+      </c>
+      <c r="P86" s="1">
+        <v>6750</v>
+      </c>
+    </row>
+    <row r="87" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J87" s="1">
+        <v>13148</v>
+      </c>
+      <c r="P87" s="1">
+        <v>6250</v>
+      </c>
+    </row>
+    <row r="88" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J88" s="1">
+        <v>12572</v>
+      </c>
+      <c r="P88" s="1">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="89" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J89" s="1">
+        <v>11789</v>
+      </c>
+      <c r="P89" s="1">
+        <v>5208</v>
+      </c>
+    </row>
+    <row r="90" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J90" s="1">
+        <v>11581</v>
+      </c>
+      <c r="P90" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="91" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J91" s="1">
+        <v>11250</v>
+      </c>
+      <c r="P91" s="1">
+        <v>4969</v>
+      </c>
+    </row>
+    <row r="92" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J92" s="1">
+        <v>10954</v>
+      </c>
+      <c r="P92" s="1">
+        <v>4521</v>
+      </c>
+    </row>
+    <row r="93" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J93" s="1">
+        <v>10816</v>
+      </c>
+      <c r="P93" s="1">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="94" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J94" s="1">
+        <v>10415</v>
+      </c>
+      <c r="P94" s="1">
+        <v>4465</v>
+      </c>
+    </row>
+    <row r="95" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J95" s="1">
+        <v>9818</v>
+      </c>
+      <c r="P95" s="1">
+        <v>2478</v>
+      </c>
+    </row>
+    <row r="96" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J96" s="1">
+        <v>9700</v>
+      </c>
+      <c r="P96" s="1">
+        <v>2125</v>
+      </c>
+    </row>
+    <row r="97" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J97" s="1">
+        <v>9500</v>
+      </c>
+      <c r="P97" s="1">
+        <v>367437</v>
+      </c>
+    </row>
+    <row r="98" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J98" s="1">
+        <v>9076</v>
+      </c>
+      <c r="P98" s="1">
+        <v>328840</v>
+      </c>
+    </row>
+    <row r="99" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J99" s="1">
+        <v>9000</v>
+      </c>
+      <c r="P99" s="1">
+        <v>272380</v>
+      </c>
+    </row>
+    <row r="100" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J100" s="1">
+        <v>8750</v>
+      </c>
+      <c r="P100" s="1">
+        <v>257088</v>
+      </c>
+    </row>
+    <row r="101" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J101" s="1">
+        <v>8750</v>
+      </c>
+      <c r="P101" s="1">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="102" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J102" s="1">
+        <v>8542</v>
+      </c>
+      <c r="P102" s="1">
+        <v>170170</v>
+      </c>
+    </row>
+    <row r="103" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J103" s="1">
+        <v>8380</v>
+      </c>
+      <c r="P103" s="1">
+        <v>155010</v>
+      </c>
+    </row>
+    <row r="104" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J104" s="1">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="105" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J105" s="1">
+        <v>7993</v>
+      </c>
+    </row>
+    <row r="106" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J106" s="1">
+        <v>7086</v>
+      </c>
+    </row>
+    <row r="107" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J107" s="1">
+        <v>7060</v>
+      </c>
+    </row>
+    <row r="108" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J108" s="1">
+        <v>6875</v>
+      </c>
+    </row>
+    <row r="109" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J109" s="1">
+        <v>6834</v>
+      </c>
+    </row>
+    <row r="110" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J110" s="1">
+        <v>6750</v>
+      </c>
+    </row>
+    <row r="111" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J111" s="1">
+        <v>6352</v>
+      </c>
+    </row>
+    <row r="112" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J112" s="1">
+        <v>6250</v>
+      </c>
+    </row>
+    <row r="113" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J113" s="1">
+        <v>5923</v>
+      </c>
+    </row>
+    <row r="114" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J114" s="1">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="115" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J115" s="1">
+        <v>5495</v>
+      </c>
+    </row>
+    <row r="116" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J116" s="1">
+        <v>5208</v>
+      </c>
+    </row>
+    <row r="117" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J117" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="118" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J118" s="1">
+        <v>4969</v>
+      </c>
+    </row>
+    <row r="119" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J119" s="1">
+        <v>4521</v>
+      </c>
+    </row>
+    <row r="120" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J120" s="1">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="121" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J121" s="1">
+        <v>4465</v>
+      </c>
+    </row>
+    <row r="122" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J122" s="1">
+        <v>3854</v>
+      </c>
+    </row>
+    <row r="123" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J123" s="1">
+        <v>3748</v>
+      </c>
+    </row>
+    <row r="124" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J124" s="1">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="125" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J125" s="1">
+        <v>2478</v>
+      </c>
+    </row>
+    <row r="126" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J126" s="1">
+        <v>2445</v>
+      </c>
+    </row>
+    <row r="127" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J127" s="1">
+        <v>2302</v>
+      </c>
+    </row>
+    <row r="128" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J128" s="1">
+        <v>2125</v>
+      </c>
+    </row>
+    <row r="129" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J129" s="1">
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="130" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J130" s="1">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="131" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J131" s="1">
+        <v>367437</v>
+      </c>
+    </row>
+    <row r="132" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J132" s="1">
+        <v>328840</v>
+      </c>
+    </row>
+    <row r="133" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J133" s="1">
+        <v>272380</v>
+      </c>
+    </row>
+    <row r="134" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J134" s="1">
+        <v>267035</v>
+      </c>
+    </row>
+    <row r="135" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J135" s="1">
+        <v>257088</v>
+      </c>
+    </row>
+    <row r="136" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J136" s="1">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="137" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J137" s="1">
+        <v>219537</v>
+      </c>
+    </row>
+    <row r="138" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J138" s="1">
+        <v>217500</v>
+      </c>
+    </row>
+    <row r="139" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J139" s="1">
+        <v>174046</v>
+      </c>
+    </row>
+    <row r="140" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J140" s="1">
+        <v>170170</v>
+      </c>
+    </row>
+    <row r="141" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J141" s="1">
+        <v>155010</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4851,7 +6218,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B59"/>
   <sheetViews>
     <sheetView topLeftCell="A37" workbookViewId="0">
@@ -5341,7 +6708,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
@@ -6009,7 +7376,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6855,22 +8222,867 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21F03872-F1FF-4113-A1D9-ED5A162594BE}">
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:J59"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="12" max="12" width="18.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2">
+        <v>117426</v>
+      </c>
+      <c r="C2">
+        <v>10524</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1204802469.8699999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>679626</v>
+      </c>
+      <c r="C3">
+        <v>55822</v>
+      </c>
+      <c r="D3" s="1">
+        <v>5535516018.1000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>378260</v>
+      </c>
+      <c r="C4">
+        <v>36880</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2853488388.9299998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>4302</v>
+      </c>
+      <c r="C5">
+        <v>290</v>
+      </c>
+      <c r="D5" s="1">
+        <v>11741698.859999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>887497</v>
+      </c>
+      <c r="C6">
+        <v>68860</v>
+      </c>
+      <c r="D6" s="1">
+        <v>7524498758.6499996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7">
+        <v>6178761</v>
+      </c>
+      <c r="C7">
+        <v>497427</v>
+      </c>
+      <c r="D7" s="1">
+        <v>58896588075.059998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8">
+        <v>885927</v>
+      </c>
+      <c r="C8">
+        <v>80562</v>
+      </c>
+      <c r="D8" s="1">
+        <v>8378656673.8699999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9">
+        <v>616411</v>
+      </c>
+      <c r="C9">
+        <v>54460</v>
+      </c>
+      <c r="D9" s="1">
+        <v>5910956662.8800001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10">
+        <v>168366</v>
+      </c>
+      <c r="C10">
+        <v>10477</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1873116776.8900001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11">
+        <v>139144</v>
+      </c>
+      <c r="C11">
+        <v>9614</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1253859541.23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12">
+        <v>3303060</v>
+      </c>
+      <c r="C12">
+        <v>325057</v>
+      </c>
+      <c r="D12" s="1">
+        <v>27049023871.610001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13">
+        <v>1493822</v>
+      </c>
+      <c r="C13">
+        <v>134358</v>
+      </c>
+      <c r="D13" s="1">
+        <v>12519505401.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <v>32124</v>
+      </c>
+      <c r="C14">
+        <v>2067</v>
+      </c>
+      <c r="D14" s="1">
+        <v>167885817.30000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15">
+        <v>226101</v>
+      </c>
+      <c r="C15">
+        <v>19054</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2017833948.4300001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16">
+        <v>529144</v>
+      </c>
+      <c r="C16">
+        <v>54253</v>
+      </c>
+      <c r="D16" s="1">
+        <v>4426504695.2299995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17">
+        <v>272600</v>
+      </c>
+      <c r="C17">
+        <v>22519</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2055312185.8599999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18">
+        <v>2217285</v>
+      </c>
+      <c r="C18">
+        <v>197824</v>
+      </c>
+      <c r="D18" s="1">
+        <v>20935034757.240002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19">
+        <v>961239</v>
+      </c>
+      <c r="C19">
+        <v>72783</v>
+      </c>
+      <c r="D19" s="1">
+        <v>8315790247.6300001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20">
+        <v>525097</v>
+      </c>
+      <c r="C20">
+        <v>49858</v>
+      </c>
+      <c r="D20" s="1">
+        <v>4594063210.5900002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>604392</v>
+      </c>
+      <c r="C21">
+        <v>46108</v>
+      </c>
+      <c r="D21" s="1">
+        <v>4864911836.1199999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22">
+        <v>811809</v>
+      </c>
+      <c r="C22">
+        <v>66558</v>
+      </c>
+      <c r="D22" s="1">
+        <v>6842643643.6400003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23">
+        <v>1177975</v>
+      </c>
+      <c r="C23">
+        <v>94164</v>
+      </c>
+      <c r="D23" s="1">
+        <v>11829456698.610001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24">
+        <v>950460</v>
+      </c>
+      <c r="C24">
+        <v>70422</v>
+      </c>
+      <c r="D24" s="1">
+        <v>8822436883.8899994</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25">
+        <v>256260</v>
+      </c>
+      <c r="C25">
+        <v>26039</v>
+      </c>
+      <c r="D25" s="1">
+        <v>2143013929.5599999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26">
+        <v>1568960</v>
+      </c>
+      <c r="C26">
+        <v>108059</v>
+      </c>
+      <c r="D26" s="1">
+        <v>14009282707.209999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27">
+        <v>1102491</v>
+      </c>
+      <c r="C27">
+        <v>88655</v>
+      </c>
+      <c r="D27" s="1">
+        <v>10220005957.99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28">
+        <v>945927</v>
+      </c>
+      <c r="C28">
+        <v>84884</v>
+      </c>
+      <c r="D28" s="1">
+        <v>7980519536.7700005</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29">
+        <v>7488</v>
+      </c>
+      <c r="C29">
+        <v>407</v>
+      </c>
+      <c r="D29" s="1">
+        <v>30261999.649999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30">
+        <v>419948</v>
+      </c>
+      <c r="C30">
+        <v>43033</v>
+      </c>
+      <c r="D30" s="1">
+        <v>2966058332.9000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31">
+        <v>217046</v>
+      </c>
+      <c r="C31">
+        <v>22239</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1694681446.6199999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32">
+        <v>1262514</v>
+      </c>
+      <c r="C32">
+        <v>98005</v>
+      </c>
+      <c r="D32" s="1">
+        <v>10048356169.719999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33">
+        <v>178084</v>
+      </c>
+      <c r="C33">
+        <v>18059</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1666936743.8199999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34">
+        <v>331823</v>
+      </c>
+      <c r="C34">
+        <v>36736</v>
+      </c>
+      <c r="D34" s="1">
+        <v>2743159070.0100002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35">
+        <v>220664</v>
+      </c>
+      <c r="C35">
+        <v>17245</v>
+      </c>
+      <c r="D35" s="1">
+        <v>2044340596.3399999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36">
+        <v>1527821</v>
+      </c>
+      <c r="C36">
+        <v>120075</v>
+      </c>
+      <c r="D36" s="1">
+        <v>14957978359.43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37">
+        <v>251346</v>
+      </c>
+      <c r="C37">
+        <v>19409</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1957766419.97</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38">
+        <v>428362</v>
+      </c>
+      <c r="C38">
+        <v>36058</v>
+      </c>
+      <c r="D38" s="1">
+        <v>3693039518.0700002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39">
+        <v>3265581</v>
+      </c>
+      <c r="C39">
+        <v>276534</v>
+      </c>
+      <c r="D39" s="1">
+        <v>33006598739.860001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40">
+        <v>1894366</v>
+      </c>
+      <c r="C40">
+        <v>130674</v>
+      </c>
+      <c r="D40" s="1">
+        <v>16761628861.389999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41">
+        <v>624341</v>
+      </c>
+      <c r="C41">
+        <v>62368</v>
+      </c>
+      <c r="D41" s="1">
+        <v>5196272103.6300001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42">
+        <v>618828</v>
+      </c>
+      <c r="C42">
+        <v>51680</v>
+      </c>
+      <c r="D42" s="1">
+        <v>5625115417.5500002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43">
+        <v>1858612</v>
+      </c>
+      <c r="C43">
+        <v>129835</v>
+      </c>
+      <c r="D43" s="1">
+        <v>17073421817.74</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44">
+        <v>386084</v>
+      </c>
+      <c r="C44">
+        <v>38521</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1784191291.6300001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45">
+        <v>161577</v>
+      </c>
+      <c r="C45">
+        <v>12447</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1461780527.77</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>15</v>
+      </c>
+      <c r="B46">
+        <v>669059</v>
+      </c>
+      <c r="C46">
+        <v>54481</v>
+      </c>
+      <c r="D46" s="1">
+        <v>5085329995.1000004</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47">
+        <v>183544</v>
+      </c>
+      <c r="C47">
+        <v>20044</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1483883396.9400001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>28</v>
+      </c>
+      <c r="B48">
+        <v>926420</v>
+      </c>
+      <c r="C48">
+        <v>75885</v>
+      </c>
+      <c r="D48" s="1">
+        <v>7621907803.5200005</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>33</v>
+      </c>
+      <c r="B49">
+        <v>4340525</v>
+      </c>
+      <c r="C49">
+        <v>350942</v>
+      </c>
+      <c r="D49" s="1">
+        <v>37610506671.25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50">
+        <v>600186</v>
+      </c>
+      <c r="C50">
+        <v>48131</v>
+      </c>
+      <c r="D50" s="1">
+        <v>5014068761.1999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51">
+        <v>985183</v>
+      </c>
+      <c r="C51">
+        <v>76101</v>
+      </c>
+      <c r="D51" s="1">
+        <v>9209253708.6599998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52">
+        <v>17130</v>
+      </c>
+      <c r="C52">
+        <v>1955</v>
+      </c>
+      <c r="D52" s="1">
+        <v>124013257.95</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>47</v>
+      </c>
+      <c r="B53">
+        <v>116841</v>
+      </c>
+      <c r="C53">
+        <v>10017</v>
+      </c>
+      <c r="D53" s="1">
+        <v>1048681417.35</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54">
+        <v>917490</v>
+      </c>
+      <c r="C54">
+        <v>79062</v>
+      </c>
+      <c r="D54" s="1">
+        <v>8830231317.0699997</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>40</v>
+      </c>
+      <c r="B55">
+        <v>1021139</v>
+      </c>
+      <c r="C55">
+        <v>77951</v>
+      </c>
+      <c r="D55" s="1">
+        <v>8751554319.4099998</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56">
+        <v>206881</v>
+      </c>
+      <c r="C56">
+        <v>16175</v>
+      </c>
+      <c r="D56" s="1">
+        <v>1656675749.5599999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>26</v>
+      </c>
+      <c r="B57">
+        <v>111633</v>
+      </c>
+      <c r="C57">
+        <v>12608</v>
+      </c>
+      <c r="D57" s="1">
+        <v>989550976.48000002</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B59">
+        <f>SUM(B2:B57)</f>
+        <v>50784982</v>
+      </c>
+      <c r="C59">
+        <f>SUM(C2:C57)</f>
+        <v>4224255</v>
+      </c>
+      <c r="D59">
+        <f>SUM(D2:D57)</f>
+        <v>452373695184.10986</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B61">
+        <v>50784982</v>
+      </c>
+      <c r="C61">
+        <v>4224255</v>
+      </c>
+      <c r="D61" s="1">
+        <v>452373695184.10999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:J63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.88671875" bestFit="1" customWidth="1"/>
@@ -8760,13 +10972,121 @@
         <v>27400</v>
       </c>
     </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>223</v>
+      </c>
+      <c r="B61" s="11">
+        <f>SUM(B2:B59)</f>
+        <v>5156850</v>
+      </c>
+      <c r="C61" s="11">
+        <f>SUM(C2:C59)</f>
+        <v>50785196</v>
+      </c>
+      <c r="D61" s="9">
+        <f>SUM(D2:D59)</f>
+        <v>522949800494.12</v>
+      </c>
+      <c r="E61" s="9">
+        <f>D61/B61</f>
+        <v>101408.76707566052</v>
+      </c>
+      <c r="F61" s="12">
+        <v>12.0222339797195</v>
+      </c>
+      <c r="G61" s="9">
+        <v>8907.6273608625088</v>
+      </c>
+      <c r="H61" s="10">
+        <f>SUM(H2:H59)</f>
+        <v>932556</v>
+      </c>
+      <c r="I61" s="9">
+        <f>SUM(I2:I59)</f>
+        <v>70573990121.259995</v>
+      </c>
+      <c r="J61" s="9">
+        <f>I61/H61</f>
+        <v>75678.018393812265</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F62" t="s">
+        <v>229</v>
+      </c>
+      <c r="G62" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H63" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62128980-318C-414D-B556-68D5E09A726A}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>50784982</v>
+      </c>
+      <c r="B2">
+        <v>4224255</v>
+      </c>
+      <c r="C2" s="1">
+        <v>452373695184.10999</v>
+      </c>
+      <c r="E2" s="2">
+        <f>A2/B2</f>
+        <v>12.0222339797195</v>
+      </c>
+      <c r="F2" s="1">
+        <f>C2/A2</f>
+        <v>8907.6273608625088</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P139"/>
   <sheetViews>
@@ -15744,7 +18064,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P139">
+  <autoFilter ref="A1:P139" xr:uid="{00000000-0009-0000-0000-000006000000}">
     <filterColumn colId="12">
       <filters>
         <filter val="NULL"/>
@@ -15753,1332 +18073,4 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:S141"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D2" t="s">
-        <v>213</v>
-      </c>
-      <c r="L2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D3" t="s">
-        <v>211</v>
-      </c>
-      <c r="E3" t="s">
-        <v>207</v>
-      </c>
-      <c r="F3" t="s">
-        <v>208</v>
-      </c>
-      <c r="G3" t="s">
-        <v>209</v>
-      </c>
-      <c r="H3" t="s">
-        <v>217</v>
-      </c>
-      <c r="J3" t="s">
-        <v>68</v>
-      </c>
-      <c r="L3" t="s">
-        <v>210</v>
-      </c>
-      <c r="M3" t="s">
-        <v>211</v>
-      </c>
-      <c r="N3" t="s">
-        <v>212</v>
-      </c>
-      <c r="P3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>148440</v>
-      </c>
-      <c r="B4">
-        <v>12</v>
-      </c>
-      <c r="D4">
-        <f>COUNT(A4:A41)</f>
-        <v>38</v>
-      </c>
-      <c r="E4" s="1">
-        <f>SUM(A4:A41)</f>
-        <v>2070510</v>
-      </c>
-      <c r="F4" s="4">
-        <f>SUM(B4:B41)</f>
-        <v>220</v>
-      </c>
-      <c r="G4" s="2">
-        <f>F4/D4</f>
-        <v>5.7894736842105265</v>
-      </c>
-      <c r="H4" s="5">
-        <f>E4/F4</f>
-        <v>9411.4090909090901</v>
-      </c>
-      <c r="J4" s="1">
-        <v>148440</v>
-      </c>
-      <c r="L4" s="1">
-        <f>SUM(J4:J141)</f>
-        <v>6030063</v>
-      </c>
-      <c r="M4">
-        <f>COUNT(J4:J141)</f>
-        <v>138</v>
-      </c>
-      <c r="N4" s="1">
-        <f>L4/M4</f>
-        <v>43696.108695652176</v>
-      </c>
-      <c r="P4" s="1">
-        <v>109988</v>
-      </c>
-      <c r="R4" s="1">
-        <f>SUM(P4:P103)</f>
-        <v>3959553</v>
-      </c>
-      <c r="S4">
-        <f>COUNT(P4:P103)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>128440</v>
-      </c>
-      <c r="B5">
-        <v>9</v>
-      </c>
-      <c r="J5" s="1">
-        <v>128440</v>
-      </c>
-      <c r="P5" s="1">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>111200</v>
-      </c>
-      <c r="B6">
-        <v>10</v>
-      </c>
-      <c r="J6" s="1">
-        <v>111200</v>
-      </c>
-      <c r="P6" s="1">
-        <v>89241</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>90394</v>
-      </c>
-      <c r="B7">
-        <v>20</v>
-      </c>
-      <c r="J7" s="1">
-        <v>109988</v>
-      </c>
-      <c r="P7" s="1">
-        <v>87886</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>62398</v>
-      </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
-      <c r="J8" s="1">
-        <v>100000</v>
-      </c>
-      <c r="P8" s="1">
-        <v>80260</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>61711</v>
-      </c>
-      <c r="B9">
-        <v>4</v>
-      </c>
-      <c r="J9" s="1">
-        <v>90394</v>
-      </c>
-      <c r="P9" s="1">
-        <v>79003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>60320</v>
-      </c>
-      <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="J10" s="1">
-        <v>89241</v>
-      </c>
-      <c r="P10" s="1">
-        <v>76871</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>52861</v>
-      </c>
-      <c r="B11">
-        <v>14</v>
-      </c>
-      <c r="J11" s="1">
-        <v>87886</v>
-      </c>
-      <c r="P11" s="1">
-        <v>57430</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>52605</v>
-      </c>
-      <c r="B12">
-        <v>6</v>
-      </c>
-      <c r="J12" s="1">
-        <v>80260</v>
-      </c>
-      <c r="P12" s="1">
-        <v>49563</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>49207</v>
-      </c>
-      <c r="B13">
-        <v>4</v>
-      </c>
-      <c r="J13" s="1">
-        <v>79003</v>
-      </c>
-      <c r="P13" s="1">
-        <v>43168</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>44129</v>
-      </c>
-      <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="J14" s="1">
-        <v>76871</v>
-      </c>
-      <c r="P14" s="1">
-        <v>41668</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>37582</v>
-      </c>
-      <c r="B15">
-        <v>8</v>
-      </c>
-      <c r="J15" s="1">
-        <v>62398</v>
-      </c>
-      <c r="P15" s="1">
-        <v>41500</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>37500</v>
-      </c>
-      <c r="B16">
-        <v>5</v>
-      </c>
-      <c r="J16" s="1">
-        <v>61711</v>
-      </c>
-      <c r="P16" s="1">
-        <v>41153</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>33233</v>
-      </c>
-      <c r="B17">
-        <v>12</v>
-      </c>
-      <c r="J17" s="1">
-        <v>60320</v>
-      </c>
-      <c r="P17" s="1">
-        <v>36723</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>30000</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="J18" s="1">
-        <v>57430</v>
-      </c>
-      <c r="P18" s="1">
-        <v>34188</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>22455</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="J19" s="1">
-        <v>52861</v>
-      </c>
-      <c r="P19" s="1">
-        <v>32625</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>21815</v>
-      </c>
-      <c r="B20">
-        <v>7</v>
-      </c>
-      <c r="J20" s="1">
-        <v>52605</v>
-      </c>
-      <c r="P20" s="1">
-        <v>31340</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>21051</v>
-      </c>
-      <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="J21" s="1">
-        <v>49563</v>
-      </c>
-      <c r="P21" s="1">
-        <v>30824</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>20274</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="J22" s="1">
-        <v>49207</v>
-      </c>
-      <c r="P22" s="1">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>16467</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="J23" s="1">
-        <v>44129</v>
-      </c>
-      <c r="P23" s="1">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>16385</v>
-      </c>
-      <c r="B24">
-        <v>4</v>
-      </c>
-      <c r="J24" s="1">
-        <v>43168</v>
-      </c>
-      <c r="P24" s="1">
-        <v>27684</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
-        <v>15000</v>
-      </c>
-      <c r="B25">
-        <v>5</v>
-      </c>
-      <c r="J25" s="1">
-        <v>41668</v>
-      </c>
-      <c r="P25" s="1">
-        <v>27427</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
-        <v>12572</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="J26" s="1">
-        <v>41500</v>
-      </c>
-      <c r="P26" s="1">
-        <v>27275</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
-        <v>10415</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="J27" s="1">
-        <v>41153</v>
-      </c>
-      <c r="P27" s="1">
-        <v>25762</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
-        <v>6352</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="J28" s="1">
-        <v>37582</v>
-      </c>
-      <c r="P28" s="1">
-        <v>23968</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
-        <v>5923</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="J29" s="1">
-        <v>37500</v>
-      </c>
-      <c r="P29" s="1">
-        <v>23021</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
-        <v>5495</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="J30" s="1">
-        <v>36723</v>
-      </c>
-      <c r="P30" s="1">
-        <v>22528</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
-        <v>3854</v>
-      </c>
-      <c r="B31">
-        <v>2</v>
-      </c>
-      <c r="J31" s="1">
-        <v>34188</v>
-      </c>
-      <c r="P31" s="1">
-        <v>22500</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A32" s="1">
-        <v>3748</v>
-      </c>
-      <c r="B32">
-        <v>2</v>
-      </c>
-      <c r="J32" s="1">
-        <v>33233</v>
-      </c>
-      <c r="P32" s="1">
-        <v>22500</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A33" s="1">
-        <v>2500</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="J33" s="1">
-        <v>32625</v>
-      </c>
-      <c r="P33" s="1">
-        <v>22200</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
-        <v>2445</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="J34" s="1">
-        <v>31340</v>
-      </c>
-      <c r="P34" s="1">
-        <v>21813</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
-        <v>2302</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="J35" s="1">
-        <v>30824</v>
-      </c>
-      <c r="P35" s="1">
-        <v>21250</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
-        <v>1987</v>
-      </c>
-      <c r="B36">
-        <v>2</v>
-      </c>
-      <c r="J36" s="1">
-        <v>30000</v>
-      </c>
-      <c r="P36" s="1">
-        <v>20833</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A37" s="1">
-        <v>1332</v>
-      </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="J37" s="1">
-        <v>30000</v>
-      </c>
-      <c r="P37" s="1">
-        <v>20833</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A38" s="1">
-        <v>267035</v>
-      </c>
-      <c r="B38">
-        <v>16</v>
-      </c>
-      <c r="J38" s="1">
-        <v>30000</v>
-      </c>
-      <c r="P38" s="1">
-        <v>20833</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A39" s="1">
-        <v>219537</v>
-      </c>
-      <c r="B39">
-        <v>17</v>
-      </c>
-      <c r="J39" s="1">
-        <v>27684</v>
-      </c>
-      <c r="P39" s="1">
-        <v>20833</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A40" s="1">
-        <v>217500</v>
-      </c>
-      <c r="B40">
-        <v>14</v>
-      </c>
-      <c r="J40" s="1">
-        <v>27427</v>
-      </c>
-      <c r="P40" s="1">
-        <v>20833</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A41" s="1">
-        <v>174046</v>
-      </c>
-      <c r="B41">
-        <v>18</v>
-      </c>
-      <c r="J41" s="1">
-        <v>27275</v>
-      </c>
-      <c r="P41" s="1">
-        <v>20691</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J42" s="1">
-        <v>25762</v>
-      </c>
-      <c r="P42" s="1">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J43" s="1">
-        <v>23968</v>
-      </c>
-      <c r="P43" s="1">
-        <v>19353</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J44" s="1">
-        <v>23021</v>
-      </c>
-      <c r="P44" s="1">
-        <v>18203</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J45" s="1">
-        <v>22528</v>
-      </c>
-      <c r="P45" s="1">
-        <v>17693</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J46" s="1">
-        <v>22500</v>
-      </c>
-      <c r="P46" s="1">
-        <v>17500</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J47" s="1">
-        <v>22500</v>
-      </c>
-      <c r="P47" s="1">
-        <v>17500</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J48" s="1">
-        <v>22455</v>
-      </c>
-      <c r="P48" s="1">
-        <v>17415</v>
-      </c>
-    </row>
-    <row r="49" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J49" s="1">
-        <v>22200</v>
-      </c>
-      <c r="P49" s="1">
-        <v>17000</v>
-      </c>
-    </row>
-    <row r="50" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J50" s="1">
-        <v>21815</v>
-      </c>
-      <c r="P50" s="1">
-        <v>16968</v>
-      </c>
-    </row>
-    <row r="51" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J51" s="1">
-        <v>21813</v>
-      </c>
-      <c r="P51" s="1">
-        <v>16873</v>
-      </c>
-    </row>
-    <row r="52" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J52" s="1">
-        <v>21250</v>
-      </c>
-      <c r="P52" s="1">
-        <v>16350</v>
-      </c>
-    </row>
-    <row r="53" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J53" s="1">
-        <v>21051</v>
-      </c>
-      <c r="P53" s="1">
-        <v>16115</v>
-      </c>
-    </row>
-    <row r="54" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J54" s="1">
-        <v>20833</v>
-      </c>
-      <c r="P54" s="1">
-        <v>15960</v>
-      </c>
-    </row>
-    <row r="55" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J55" s="1">
-        <v>20833</v>
-      </c>
-      <c r="P55" s="1">
-        <v>15870</v>
-      </c>
-    </row>
-    <row r="56" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J56" s="1">
-        <v>20833</v>
-      </c>
-      <c r="P56" s="1">
-        <v>15625</v>
-      </c>
-    </row>
-    <row r="57" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J57" s="1">
-        <v>20833</v>
-      </c>
-      <c r="P57" s="1">
-        <v>15433</v>
-      </c>
-    </row>
-    <row r="58" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J58" s="1">
-        <v>20833</v>
-      </c>
-      <c r="P58" s="1">
-        <v>15291</v>
-      </c>
-    </row>
-    <row r="59" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J59" s="1">
-        <v>20691</v>
-      </c>
-      <c r="P59" s="1">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="60" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J60" s="1">
-        <v>20274</v>
-      </c>
-      <c r="P60" s="1">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="61" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J61" s="1">
-        <v>20000</v>
-      </c>
-      <c r="P61" s="1">
-        <v>14603</v>
-      </c>
-    </row>
-    <row r="62" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J62" s="1">
-        <v>19353</v>
-      </c>
-      <c r="P62" s="1">
-        <v>14543</v>
-      </c>
-    </row>
-    <row r="63" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J63" s="1">
-        <v>18203</v>
-      </c>
-      <c r="P63" s="1">
-        <v>14282</v>
-      </c>
-    </row>
-    <row r="64" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J64" s="1">
-        <v>17693</v>
-      </c>
-      <c r="P64" s="1">
-        <v>13168</v>
-      </c>
-    </row>
-    <row r="65" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J65" s="1">
-        <v>17500</v>
-      </c>
-      <c r="P65" s="1">
-        <v>13148</v>
-      </c>
-    </row>
-    <row r="66" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J66" s="1">
-        <v>17500</v>
-      </c>
-      <c r="P66" s="1">
-        <v>11789</v>
-      </c>
-    </row>
-    <row r="67" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J67" s="1">
-        <v>17415</v>
-      </c>
-      <c r="P67" s="1">
-        <v>11581</v>
-      </c>
-    </row>
-    <row r="68" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J68" s="1">
-        <v>17000</v>
-      </c>
-      <c r="P68" s="1">
-        <v>11250</v>
-      </c>
-    </row>
-    <row r="69" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J69" s="1">
-        <v>16968</v>
-      </c>
-      <c r="P69" s="1">
-        <v>10954</v>
-      </c>
-    </row>
-    <row r="70" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J70" s="1">
-        <v>16873</v>
-      </c>
-      <c r="P70" s="1">
-        <v>10816</v>
-      </c>
-    </row>
-    <row r="71" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J71" s="1">
-        <v>16467</v>
-      </c>
-      <c r="P71" s="1">
-        <v>9818</v>
-      </c>
-    </row>
-    <row r="72" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J72" s="1">
-        <v>16385</v>
-      </c>
-      <c r="P72" s="1">
-        <v>9700</v>
-      </c>
-    </row>
-    <row r="73" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J73" s="1">
-        <v>16350</v>
-      </c>
-      <c r="P73" s="1">
-        <v>9500</v>
-      </c>
-    </row>
-    <row r="74" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J74" s="1">
-        <v>16115</v>
-      </c>
-      <c r="P74" s="1">
-        <v>9076</v>
-      </c>
-    </row>
-    <row r="75" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J75" s="1">
-        <v>15960</v>
-      </c>
-      <c r="P75" s="1">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="76" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J76" s="1">
-        <v>15870</v>
-      </c>
-      <c r="P76" s="1">
-        <v>8750</v>
-      </c>
-    </row>
-    <row r="77" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J77" s="1">
-        <v>15625</v>
-      </c>
-      <c r="P77" s="1">
-        <v>8750</v>
-      </c>
-    </row>
-    <row r="78" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J78" s="1">
-        <v>15433</v>
-      </c>
-      <c r="P78" s="1">
-        <v>8542</v>
-      </c>
-    </row>
-    <row r="79" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J79" s="1">
-        <v>15291</v>
-      </c>
-      <c r="P79" s="1">
-        <v>8380</v>
-      </c>
-    </row>
-    <row r="80" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J80" s="1">
-        <v>15000</v>
-      </c>
-      <c r="P80" s="1">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="81" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J81" s="1">
-        <v>15000</v>
-      </c>
-      <c r="P81" s="1">
-        <v>7993</v>
-      </c>
-    </row>
-    <row r="82" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J82" s="1">
-        <v>15000</v>
-      </c>
-      <c r="P82" s="1">
-        <v>7086</v>
-      </c>
-    </row>
-    <row r="83" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J83" s="1">
-        <v>14603</v>
-      </c>
-      <c r="P83" s="1">
-        <v>7060</v>
-      </c>
-    </row>
-    <row r="84" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J84" s="1">
-        <v>14543</v>
-      </c>
-      <c r="P84" s="1">
-        <v>6875</v>
-      </c>
-    </row>
-    <row r="85" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J85" s="1">
-        <v>14282</v>
-      </c>
-      <c r="P85" s="1">
-        <v>6834</v>
-      </c>
-    </row>
-    <row r="86" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J86" s="1">
-        <v>13168</v>
-      </c>
-      <c r="P86" s="1">
-        <v>6750</v>
-      </c>
-    </row>
-    <row r="87" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J87" s="1">
-        <v>13148</v>
-      </c>
-      <c r="P87" s="1">
-        <v>6250</v>
-      </c>
-    </row>
-    <row r="88" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J88" s="1">
-        <v>12572</v>
-      </c>
-      <c r="P88" s="1">
-        <v>5500</v>
-      </c>
-    </row>
-    <row r="89" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J89" s="1">
-        <v>11789</v>
-      </c>
-      <c r="P89" s="1">
-        <v>5208</v>
-      </c>
-    </row>
-    <row r="90" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J90" s="1">
-        <v>11581</v>
-      </c>
-      <c r="P90" s="1">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="91" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J91" s="1">
-        <v>11250</v>
-      </c>
-      <c r="P91" s="1">
-        <v>4969</v>
-      </c>
-    </row>
-    <row r="92" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J92" s="1">
-        <v>10954</v>
-      </c>
-      <c r="P92" s="1">
-        <v>4521</v>
-      </c>
-    </row>
-    <row r="93" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J93" s="1">
-        <v>10816</v>
-      </c>
-      <c r="P93" s="1">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="94" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J94" s="1">
-        <v>10415</v>
-      </c>
-      <c r="P94" s="1">
-        <v>4465</v>
-      </c>
-    </row>
-    <row r="95" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J95" s="1">
-        <v>9818</v>
-      </c>
-      <c r="P95" s="1">
-        <v>2478</v>
-      </c>
-    </row>
-    <row r="96" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J96" s="1">
-        <v>9700</v>
-      </c>
-      <c r="P96" s="1">
-        <v>2125</v>
-      </c>
-    </row>
-    <row r="97" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J97" s="1">
-        <v>9500</v>
-      </c>
-      <c r="P97" s="1">
-        <v>367437</v>
-      </c>
-    </row>
-    <row r="98" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J98" s="1">
-        <v>9076</v>
-      </c>
-      <c r="P98" s="1">
-        <v>328840</v>
-      </c>
-    </row>
-    <row r="99" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J99" s="1">
-        <v>9000</v>
-      </c>
-      <c r="P99" s="1">
-        <v>272380</v>
-      </c>
-    </row>
-    <row r="100" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J100" s="1">
-        <v>8750</v>
-      </c>
-      <c r="P100" s="1">
-        <v>257088</v>
-      </c>
-    </row>
-    <row r="101" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J101" s="1">
-        <v>8750</v>
-      </c>
-      <c r="P101" s="1">
-        <v>250000</v>
-      </c>
-    </row>
-    <row r="102" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J102" s="1">
-        <v>8542</v>
-      </c>
-      <c r="P102" s="1">
-        <v>170170</v>
-      </c>
-    </row>
-    <row r="103" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J103" s="1">
-        <v>8380</v>
-      </c>
-      <c r="P103" s="1">
-        <v>155010</v>
-      </c>
-    </row>
-    <row r="104" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J104" s="1">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="105" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J105" s="1">
-        <v>7993</v>
-      </c>
-    </row>
-    <row r="106" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J106" s="1">
-        <v>7086</v>
-      </c>
-    </row>
-    <row r="107" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J107" s="1">
-        <v>7060</v>
-      </c>
-    </row>
-    <row r="108" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J108" s="1">
-        <v>6875</v>
-      </c>
-    </row>
-    <row r="109" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J109" s="1">
-        <v>6834</v>
-      </c>
-    </row>
-    <row r="110" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J110" s="1">
-        <v>6750</v>
-      </c>
-    </row>
-    <row r="111" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J111" s="1">
-        <v>6352</v>
-      </c>
-    </row>
-    <row r="112" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J112" s="1">
-        <v>6250</v>
-      </c>
-    </row>
-    <row r="113" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J113" s="1">
-        <v>5923</v>
-      </c>
-    </row>
-    <row r="114" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J114" s="1">
-        <v>5500</v>
-      </c>
-    </row>
-    <row r="115" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J115" s="1">
-        <v>5495</v>
-      </c>
-    </row>
-    <row r="116" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J116" s="1">
-        <v>5208</v>
-      </c>
-    </row>
-    <row r="117" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J117" s="1">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="118" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J118" s="1">
-        <v>4969</v>
-      </c>
-    </row>
-    <row r="119" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J119" s="1">
-        <v>4521</v>
-      </c>
-    </row>
-    <row r="120" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J120" s="1">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="121" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J121" s="1">
-        <v>4465</v>
-      </c>
-    </row>
-    <row r="122" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J122" s="1">
-        <v>3854</v>
-      </c>
-    </row>
-    <row r="123" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J123" s="1">
-        <v>3748</v>
-      </c>
-    </row>
-    <row r="124" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J124" s="1">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="125" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J125" s="1">
-        <v>2478</v>
-      </c>
-    </row>
-    <row r="126" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J126" s="1">
-        <v>2445</v>
-      </c>
-    </row>
-    <row r="127" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J127" s="1">
-        <v>2302</v>
-      </c>
-    </row>
-    <row r="128" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J128" s="1">
-        <v>2125</v>
-      </c>
-    </row>
-    <row r="129" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J129" s="1">
-        <v>1987</v>
-      </c>
-    </row>
-    <row r="130" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J130" s="1">
-        <v>1332</v>
-      </c>
-    </row>
-    <row r="131" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J131" s="1">
-        <v>367437</v>
-      </c>
-    </row>
-    <row r="132" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J132" s="1">
-        <v>328840</v>
-      </c>
-    </row>
-    <row r="133" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J133" s="1">
-        <v>272380</v>
-      </c>
-    </row>
-    <row r="134" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J134" s="1">
-        <v>267035</v>
-      </c>
-    </row>
-    <row r="135" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J135" s="1">
-        <v>257088</v>
-      </c>
-    </row>
-    <row r="136" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J136" s="1">
-        <v>250000</v>
-      </c>
-    </row>
-    <row r="137" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J137" s="1">
-        <v>219537</v>
-      </c>
-    </row>
-    <row r="138" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J138" s="1">
-        <v>217500</v>
-      </c>
-    </row>
-    <row r="139" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J139" s="1">
-        <v>174046</v>
-      </c>
-    </row>
-    <row r="140" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J140" s="1">
-        <v>170170</v>
-      </c>
-    </row>
-    <row r="141" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J141" s="1">
-        <v>155010</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>